<commit_message>
Editing stats code and csvs
</commit_message>
<xml_diff>
--- a/stat_tests/combined_blocktarget_data.xlsx
+++ b/stat_tests/combined_blocktarget_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yasminebassil/Documents/Emory/3_Research/Projects/CogMap_Paper/stat_tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{3223E2C9-DB48-9C42-A177-64487B5BD7D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{59E6F97D-9061-4648-8026-5E26FA52FB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15760" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="combined_blocktarget_data" sheetId="1" r:id="rId1"/>
@@ -640,7 +640,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="30">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -733,11 +733,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -753,71 +753,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -853,56 +793,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -918,16 +808,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -963,11 +843,101 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1283,7 +1253,7 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="192" workbookViewId="0">
+    <sheetView topLeftCell="A70" zoomScale="192" workbookViewId="0">
       <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
@@ -5688,16 +5658,16 @@
     <sortCondition ref="B2:B169"/>
   </sortState>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="30" priority="3" operator="between">
-      <formula>0.05</formula>
-      <formula>0.01</formula>
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="lessThan">
+      <formula>0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="between">
       <formula>0.01</formula>
       <formula>0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="lessThan">
-      <formula>0.001</formula>
+    <cfRule type="cellIs" dxfId="27" priority="3" operator="between">
+      <formula>0.05</formula>
+      <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6288,14 +6258,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:G22">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="lessThan">
       <formula>0.001</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="25" priority="2" operator="between">
       <formula>0.01</formula>
       <formula>0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="24" priority="3" operator="between">
       <formula>0.05</formula>
       <formula>0.01</formula>
     </cfRule>
@@ -6308,8 +6278,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AF0576F-1A18-A14E-95E5-05FF9F4682C7}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView zoomScale="134" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6888,14 +6858,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G22">
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="lessThan">
       <formula>0.001</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="22" priority="5" operator="between">
       <formula>0.01</formula>
       <formula>0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="6" operator="between">
       <formula>0.05</formula>
       <formula>0.01</formula>
     </cfRule>
@@ -6921,8 +6891,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86BCC3F8-6BDA-474A-9BFE-05B009A52F83}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="218" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView zoomScale="138" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7501,14 +7471,627 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G22">
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="lessThan">
       <formula>0.001</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="16" priority="5" operator="between">
       <formula>0.01</formula>
       <formula>0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="between">
+      <formula>0.05</formula>
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="lessThan">
+      <formula>0.001</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="between">
+      <formula>0.01</formula>
+      <formula>0.001</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="between">
+      <formula>0.05</formula>
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4BCCE8-E661-0641-9B09-39215520F283}">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" zoomScale="188" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <v>17.274527379999999</v>
+      </c>
+      <c r="D2">
+        <v>9.7577998239999992</v>
+      </c>
+      <c r="E2">
+        <v>575</v>
+      </c>
+      <c r="F2">
+        <v>1.7703301659999999</v>
+      </c>
+      <c r="G2">
+        <v>0.180534417</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>26.814940870000001</v>
+      </c>
+      <c r="D3">
+        <v>9.7577998239999992</v>
+      </c>
+      <c r="E3">
+        <v>575</v>
+      </c>
+      <c r="F3">
+        <v>2.7480519540000001</v>
+      </c>
+      <c r="G3">
+        <v>1.6990379999999999E-2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>9.5404134880000004</v>
+      </c>
+      <c r="D4">
+        <v>9.7577998239999992</v>
+      </c>
+      <c r="E4">
+        <v>575</v>
+      </c>
+      <c r="F4">
+        <v>0.97772178799999998</v>
+      </c>
+      <c r="G4">
+        <v>0.59125787399999996</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>43.666612039999997</v>
+      </c>
+      <c r="D5">
+        <v>57.429401380000002</v>
+      </c>
+      <c r="E5">
+        <v>575</v>
+      </c>
+      <c r="F5">
+        <v>0.76035290300000002</v>
+      </c>
+      <c r="G5">
+        <v>0.72747204499999996</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>90.927150040000001</v>
+      </c>
+      <c r="D6">
+        <v>57.429401380000002</v>
+      </c>
+      <c r="E6">
+        <v>575</v>
+      </c>
+      <c r="F6">
+        <v>1.5832857010000001</v>
+      </c>
+      <c r="G6">
+        <v>0.25367287799999999</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>47.260537999999997</v>
+      </c>
+      <c r="D7">
+        <v>57.429401380000002</v>
+      </c>
+      <c r="E7">
+        <v>575</v>
+      </c>
+      <c r="F7">
+        <v>0.82293279900000005</v>
+      </c>
+      <c r="G7">
+        <v>0.68894245499999995</v>
+      </c>
+      <c r="H7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>0.24460538400000001</v>
+      </c>
+      <c r="D8">
+        <v>7.7646688000000005E-2</v>
+      </c>
+      <c r="E8">
+        <v>575</v>
+      </c>
+      <c r="F8">
+        <v>3.1502358880000001</v>
+      </c>
+      <c r="G8">
+        <v>4.8777880000000001E-3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>0.38608783899999999</v>
+      </c>
+      <c r="D9">
+        <v>7.7646688000000005E-2</v>
+      </c>
+      <c r="E9">
+        <v>575</v>
+      </c>
+      <c r="F9">
+        <v>4.9723670990000004</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2.61E-6</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>0.14148245400000001</v>
+      </c>
+      <c r="D10">
+        <v>7.7646688000000005E-2</v>
+      </c>
+      <c r="E10">
+        <v>575</v>
+      </c>
+      <c r="F10">
+        <v>1.82213121</v>
+      </c>
+      <c r="G10">
+        <v>0.16324422299999999</v>
+      </c>
+      <c r="H10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>16.920158579999999</v>
+      </c>
+      <c r="D11">
+        <v>9.7223171730000004</v>
+      </c>
+      <c r="E11">
+        <v>575</v>
+      </c>
+      <c r="F11">
+        <v>1.740342171</v>
+      </c>
+      <c r="G11">
+        <v>0.19112388899999999</v>
+      </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>26.206760150000001</v>
+      </c>
+      <c r="D12">
+        <v>9.7223171730000004</v>
+      </c>
+      <c r="E12">
+        <v>575</v>
+      </c>
+      <c r="F12">
+        <v>2.6955261469999998</v>
+      </c>
+      <c r="G12">
+        <v>1.9766855999999999E-2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>9.2866015730000004</v>
+      </c>
+      <c r="D13">
+        <v>9.7223171730000004</v>
+      </c>
+      <c r="E13">
+        <v>575</v>
+      </c>
+      <c r="F13">
+        <v>0.95518397600000005</v>
+      </c>
+      <c r="G13">
+        <v>0.60554817500000002</v>
+      </c>
+      <c r="H13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>0.35436880799999998</v>
+      </c>
+      <c r="D14">
+        <v>0.57008712699999997</v>
+      </c>
+      <c r="E14">
+        <v>575</v>
+      </c>
+      <c r="F14">
+        <v>0.62160464800000004</v>
+      </c>
+      <c r="G14">
+        <v>0.80833644500000001</v>
+      </c>
+      <c r="H14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>0.60818072300000003</v>
+      </c>
+      <c r="D15">
+        <v>0.57008712699999997</v>
+      </c>
+      <c r="E15">
+        <v>575</v>
+      </c>
+      <c r="F15">
+        <v>1.066820656</v>
+      </c>
+      <c r="G15">
+        <v>0.53510042899999999</v>
+      </c>
+      <c r="H15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>0.253811915</v>
+      </c>
+      <c r="D16">
+        <v>0.57008712699999997</v>
+      </c>
+      <c r="E16">
+        <v>575</v>
+      </c>
+      <c r="F16">
+        <v>0.44521600900000002</v>
+      </c>
+      <c r="G16">
+        <v>0.89653641500000003</v>
+      </c>
+      <c r="H16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>-1.8143353900000001</v>
+      </c>
+      <c r="D17">
+        <v>1.308326594</v>
+      </c>
+      <c r="E17">
+        <v>575</v>
+      </c>
+      <c r="F17">
+        <v>-1.3867603079999999</v>
+      </c>
+      <c r="G17">
+        <v>0.34849749200000002</v>
+      </c>
+      <c r="H17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>-5.3616183880000001</v>
+      </c>
+      <c r="D18">
+        <v>1.308326594</v>
+      </c>
+      <c r="E18">
+        <v>575</v>
+      </c>
+      <c r="F18">
+        <v>-4.0980733809999998</v>
+      </c>
+      <c r="G18">
+        <v>1.40844E-4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>-3.547282998</v>
+      </c>
+      <c r="D19">
+        <v>1.308326594</v>
+      </c>
+      <c r="E19">
+        <v>575</v>
+      </c>
+      <c r="F19">
+        <v>-2.7113130729999999</v>
+      </c>
+      <c r="G19">
+        <v>1.8893158E-2</v>
+      </c>
+      <c r="H19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20">
+        <v>3.269230769</v>
+      </c>
+      <c r="D20">
+        <v>9.5136111840000002</v>
+      </c>
+      <c r="E20">
+        <v>575</v>
+      </c>
+      <c r="F20">
+        <v>0.34363720599999997</v>
+      </c>
+      <c r="G20">
+        <v>0.93699168300000002</v>
+      </c>
+      <c r="H20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <v>9.5136111840000002</v>
+      </c>
+      <c r="E21">
+        <v>575</v>
+      </c>
+      <c r="F21">
+        <v>1.15623813</v>
+      </c>
+      <c r="G21">
+        <v>0.47994827800000001</v>
+      </c>
+      <c r="H21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>7.730769231</v>
+      </c>
+      <c r="D22">
+        <v>9.5136111840000002</v>
+      </c>
+      <c r="E22">
+        <v>575</v>
+      </c>
+      <c r="F22">
+        <v>0.81260092299999998</v>
+      </c>
+      <c r="G22">
+        <v>0.69536455600000002</v>
+      </c>
+      <c r="H22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G2:G22">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="lessThan">
+      <formula>0.001</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="between">
+      <formula>0.01</formula>
+      <formula>0.001</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="6" operator="between">
       <formula>0.05</formula>
       <formula>0.01</formula>
     </cfRule>
@@ -7530,12 +8113,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE4BCCE8-E661-0641-9B09-39215520F283}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D58F2A-854F-A844-90AE-65172D18A420}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="188" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7571,10 +8154,10 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2">
-        <v>17.274527379999999</v>
+        <v>10.38696507</v>
       </c>
       <c r="D2">
         <v>9.7577998239999992</v>
@@ -7583,10 +8166,10 @@
         <v>575</v>
       </c>
       <c r="F2">
-        <v>1.7703301659999999</v>
+        <v>1.064478187</v>
       </c>
       <c r="G2">
-        <v>0.180534417</v>
+        <v>0.53656520299999999</v>
       </c>
       <c r="H2" t="s">
         <v>10</v>
@@ -7597,10 +8180,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3">
-        <v>26.814940870000001</v>
+        <v>14.41384738</v>
       </c>
       <c r="D3">
         <v>9.7577998239999992</v>
@@ -7609,10 +8192,10 @@
         <v>575</v>
       </c>
       <c r="F3">
-        <v>2.7480519540000001</v>
+        <v>1.477161618</v>
       </c>
       <c r="G3">
-        <v>1.6990379999999999E-2</v>
+        <v>0.30266618000000001</v>
       </c>
       <c r="H3" t="s">
         <v>10</v>
@@ -7623,10 +8206,10 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C4">
-        <v>9.5404134880000004</v>
+        <v>4.0268823149999999</v>
       </c>
       <c r="D4">
         <v>9.7577998239999992</v>
@@ -7635,10 +8218,10 @@
         <v>575</v>
       </c>
       <c r="F4">
-        <v>0.97772178799999998</v>
+        <v>0.41268343200000002</v>
       </c>
       <c r="G4">
-        <v>0.59125787399999996</v>
+        <v>0.91042262699999998</v>
       </c>
       <c r="H4" t="s">
         <v>10</v>
@@ -7649,10 +8232,10 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5">
-        <v>43.666612039999997</v>
+        <v>32.019606680000003</v>
       </c>
       <c r="D5">
         <v>57.429401380000002</v>
@@ -7661,10 +8244,10 @@
         <v>575</v>
       </c>
       <c r="F5">
-        <v>0.76035290300000002</v>
+        <v>0.557547283</v>
       </c>
       <c r="G5">
-        <v>0.72747204499999996</v>
+        <v>0.84263443699999996</v>
       </c>
       <c r="H5" t="s">
         <v>20</v>
@@ -7675,10 +8258,10 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C6">
-        <v>90.927150040000001</v>
+        <v>48.295181020000001</v>
       </c>
       <c r="D6">
         <v>57.429401380000002</v>
@@ -7687,10 +8270,10 @@
         <v>575</v>
       </c>
       <c r="F6">
-        <v>1.5832857010000001</v>
+        <v>0.84094871000000004</v>
       </c>
       <c r="G6">
-        <v>0.25367287799999999</v>
+        <v>0.67769716700000004</v>
       </c>
       <c r="H6" t="s">
         <v>20</v>
@@ -7701,10 +8284,10 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C7">
-        <v>47.260537999999997</v>
+        <v>16.275574339999999</v>
       </c>
       <c r="D7">
         <v>57.429401380000002</v>
@@ -7713,10 +8296,10 @@
         <v>575</v>
       </c>
       <c r="F7">
-        <v>0.82293279900000005</v>
+        <v>0.28340142800000001</v>
       </c>
       <c r="G7">
-        <v>0.68894245499999995</v>
+        <v>0.95669581299999995</v>
       </c>
       <c r="H7" t="s">
         <v>20</v>
@@ -7727,10 +8310,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C8">
-        <v>0.24460538400000001</v>
+        <v>0.21669601199999999</v>
       </c>
       <c r="D8">
         <v>7.7646688000000005E-2</v>
@@ -7739,10 +8322,10 @@
         <v>575</v>
       </c>
       <c r="F8">
-        <v>3.1502358880000001</v>
+        <v>2.7907952869999999</v>
       </c>
       <c r="G8">
-        <v>4.8777880000000001E-3</v>
+        <v>1.4991436E-2</v>
       </c>
       <c r="H8" t="s">
         <v>21</v>
@@ -7753,10 +8336,10 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C9">
-        <v>0.38608783899999999</v>
+        <v>0.281123489</v>
       </c>
       <c r="D9">
         <v>7.7646688000000005E-2</v>
@@ -7765,10 +8348,10 @@
         <v>575</v>
       </c>
       <c r="F9">
-        <v>4.9723670990000004</v>
-      </c>
-      <c r="G9" s="1">
-        <v>2.61E-6</v>
+        <v>3.620547052</v>
+      </c>
+      <c r="G9">
+        <v>9.3213699999999998E-4</v>
       </c>
       <c r="H9" t="s">
         <v>21</v>
@@ -7779,10 +8362,10 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C10">
-        <v>0.14148245400000001</v>
+        <v>6.4427476999999997E-2</v>
       </c>
       <c r="D10">
         <v>7.7646688000000005E-2</v>
@@ -7791,10 +8374,10 @@
         <v>575</v>
       </c>
       <c r="F10">
-        <v>1.82213121</v>
+        <v>0.82975176500000003</v>
       </c>
       <c r="G10">
-        <v>0.16324422299999999</v>
+        <v>0.68469282799999998</v>
       </c>
       <c r="H10" t="s">
         <v>21</v>
@@ -7805,10 +8388,10 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C11">
-        <v>16.920158579999999</v>
+        <v>8.5700772080000007</v>
       </c>
       <c r="D11">
         <v>9.7223171730000004</v>
@@ -7817,10 +8400,10 @@
         <v>575</v>
       </c>
       <c r="F11">
-        <v>1.740342171</v>
+        <v>0.88148504699999997</v>
       </c>
       <c r="G11">
-        <v>0.19112388899999999</v>
+        <v>0.65221859699999996</v>
       </c>
       <c r="H11" t="s">
         <v>22</v>
@@ -7831,10 +8414,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C12">
-        <v>26.206760150000001</v>
+        <v>12.40503958</v>
       </c>
       <c r="D12">
         <v>9.7223171730000004</v>
@@ -7843,10 +8426,10 @@
         <v>575</v>
       </c>
       <c r="F12">
-        <v>2.6955261469999998</v>
+        <v>1.2759344669999999</v>
       </c>
       <c r="G12">
-        <v>1.9766855999999999E-2</v>
+        <v>0.40936276799999999</v>
       </c>
       <c r="H12" t="s">
         <v>22</v>
@@ -7857,10 +8440,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C13">
-        <v>9.2866015730000004</v>
+        <v>3.8349623689999999</v>
       </c>
       <c r="D13">
         <v>9.7223171730000004</v>
@@ -7869,10 +8452,10 @@
         <v>575</v>
       </c>
       <c r="F13">
-        <v>0.95518397600000005</v>
+        <v>0.39444942</v>
       </c>
       <c r="G13">
-        <v>0.60554817500000002</v>
+        <v>0.91783244600000002</v>
       </c>
       <c r="H13" t="s">
         <v>22</v>
@@ -7883,10 +8466,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C14">
-        <v>0.35436880799999998</v>
+        <v>1.8168878580000001</v>
       </c>
       <c r="D14">
         <v>0.57008712699999997</v>
@@ -7895,10 +8478,10 @@
         <v>575</v>
       </c>
       <c r="F14">
-        <v>0.62160464800000004</v>
+        <v>3.187035405</v>
       </c>
       <c r="G14">
-        <v>0.80833644500000001</v>
+        <v>4.3177270000000004E-3</v>
       </c>
       <c r="H14" t="s">
         <v>23</v>
@@ -7909,10 +8492,10 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C15">
-        <v>0.60818072300000003</v>
+        <v>2.0088078039999999</v>
       </c>
       <c r="D15">
         <v>0.57008712699999997</v>
@@ -7921,10 +8504,10 @@
         <v>575</v>
       </c>
       <c r="F15">
-        <v>1.066820656</v>
+        <v>3.5236856059999999</v>
       </c>
       <c r="G15">
-        <v>0.53510042899999999</v>
+        <v>1.333112E-3</v>
       </c>
       <c r="H15" t="s">
         <v>23</v>
@@ -7935,10 +8518,10 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C16">
-        <v>0.253811915</v>
+        <v>0.19191994600000001</v>
       </c>
       <c r="D16">
         <v>0.57008712699999997</v>
@@ -7947,10 +8530,10 @@
         <v>575</v>
       </c>
       <c r="F16">
-        <v>0.44521600900000002</v>
+        <v>0.33665020099999998</v>
       </c>
       <c r="G16">
-        <v>0.89653641500000003</v>
+        <v>0.93944859599999997</v>
       </c>
       <c r="H16" t="s">
         <v>23</v>
@@ -7961,10 +8544,10 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C17">
-        <v>-1.8143353900000001</v>
+        <v>-4.4100175019999996</v>
       </c>
       <c r="D17">
         <v>1.308326594</v>
@@ -7973,10 +8556,10 @@
         <v>575</v>
       </c>
       <c r="F17">
-        <v>-1.3867603079999999</v>
+        <v>-3.3707313769999998</v>
       </c>
       <c r="G17">
-        <v>0.34849749200000002</v>
+        <v>2.3040999999999999E-3</v>
       </c>
       <c r="H17" t="s">
         <v>24</v>
@@ -7987,10 +8570,10 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C18">
-        <v>-5.3616183880000001</v>
+        <v>-7.2723542490000002</v>
       </c>
       <c r="D18">
         <v>1.308326594</v>
@@ -7999,10 +8582,10 @@
         <v>575</v>
       </c>
       <c r="F18">
-        <v>-4.0980733809999998</v>
-      </c>
-      <c r="G18">
-        <v>1.40844E-4</v>
+        <v>-5.5585159559999999</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1.2499999999999999E-7</v>
       </c>
       <c r="H18" t="s">
         <v>24</v>
@@ -8013,10 +8596,10 @@
         <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C19">
-        <v>-3.547282998</v>
+        <v>-2.862336746</v>
       </c>
       <c r="D19">
         <v>1.308326594</v>
@@ -8025,10 +8608,10 @@
         <v>575</v>
       </c>
       <c r="F19">
-        <v>-2.7113130729999999</v>
+        <v>-2.1877845790000001</v>
       </c>
       <c r="G19">
-        <v>1.8893158E-2</v>
+        <v>7.4114450999999998E-2</v>
       </c>
       <c r="H19" t="s">
         <v>24</v>
@@ -8039,10 +8622,10 @@
         <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C20">
-        <v>3.269230769</v>
+        <v>4.769230769</v>
       </c>
       <c r="D20">
         <v>9.5136111840000002</v>
@@ -8051,10 +8634,10 @@
         <v>575</v>
       </c>
       <c r="F20">
-        <v>0.34363720599999997</v>
+        <v>0.50130604199999995</v>
       </c>
       <c r="G20">
-        <v>0.93699168300000002</v>
+        <v>0.87070999900000001</v>
       </c>
       <c r="H20" t="s">
         <v>25</v>
@@ -8065,10 +8648,10 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C21">
-        <v>11</v>
+        <v>6.461538462</v>
       </c>
       <c r="D21">
         <v>9.5136111840000002</v>
@@ -8077,10 +8660,10 @@
         <v>575</v>
       </c>
       <c r="F21">
-        <v>1.15623813</v>
+        <v>0.67918883100000005</v>
       </c>
       <c r="G21">
-        <v>0.47994827800000001</v>
+        <v>0.77571718999999995</v>
       </c>
       <c r="H21" t="s">
         <v>25</v>
@@ -8091,10 +8674,10 @@
         <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C22">
-        <v>7.730769231</v>
+        <v>1.692307692</v>
       </c>
       <c r="D22">
         <v>9.5136111840000002</v>
@@ -8103,10 +8686,10 @@
         <v>575</v>
       </c>
       <c r="F22">
-        <v>0.81260092299999998</v>
+        <v>0.17788278900000001</v>
       </c>
       <c r="G22">
-        <v>0.69536455600000002</v>
+        <v>0.98270765100000002</v>
       </c>
       <c r="H22" t="s">
         <v>25</v>
@@ -8114,627 +8697,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G22">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
       <formula>0.01</formula>
       <formula>0.001</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="between">
-      <formula>0.05</formula>
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
-      <formula>0.001</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
-      <formula>0.01</formula>
-      <formula>0.001</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="between">
-      <formula>0.05</formula>
-      <formula>0.01</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D58F2A-854F-A844-90AE-65172D18A420}">
-  <dimension ref="A1:H22"/>
-  <sheetViews>
-    <sheetView topLeftCell="B7" zoomScale="200" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2">
-        <v>10.38696507</v>
-      </c>
-      <c r="D2">
-        <v>9.7577998239999992</v>
-      </c>
-      <c r="E2">
-        <v>575</v>
-      </c>
-      <c r="F2">
-        <v>1.064478187</v>
-      </c>
-      <c r="G2">
-        <v>0.53656520299999999</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3">
-        <v>14.41384738</v>
-      </c>
-      <c r="D3">
-        <v>9.7577998239999992</v>
-      </c>
-      <c r="E3">
-        <v>575</v>
-      </c>
-      <c r="F3">
-        <v>1.477161618</v>
-      </c>
-      <c r="G3">
-        <v>0.30266618000000001</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4">
-        <v>4.0268823149999999</v>
-      </c>
-      <c r="D4">
-        <v>9.7577998239999992</v>
-      </c>
-      <c r="E4">
-        <v>575</v>
-      </c>
-      <c r="F4">
-        <v>0.41268343200000002</v>
-      </c>
-      <c r="G4">
-        <v>0.91042262699999998</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5">
-        <v>32.019606680000003</v>
-      </c>
-      <c r="D5">
-        <v>57.429401380000002</v>
-      </c>
-      <c r="E5">
-        <v>575</v>
-      </c>
-      <c r="F5">
-        <v>0.557547283</v>
-      </c>
-      <c r="G5">
-        <v>0.84263443699999996</v>
-      </c>
-      <c r="H5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6">
-        <v>48.295181020000001</v>
-      </c>
-      <c r="D6">
-        <v>57.429401380000002</v>
-      </c>
-      <c r="E6">
-        <v>575</v>
-      </c>
-      <c r="F6">
-        <v>0.84094871000000004</v>
-      </c>
-      <c r="G6">
-        <v>0.67769716700000004</v>
-      </c>
-      <c r="H6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7">
-        <v>16.275574339999999</v>
-      </c>
-      <c r="D7">
-        <v>57.429401380000002</v>
-      </c>
-      <c r="E7">
-        <v>575</v>
-      </c>
-      <c r="F7">
-        <v>0.28340142800000001</v>
-      </c>
-      <c r="G7">
-        <v>0.95669581299999995</v>
-      </c>
-      <c r="H7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8">
-        <v>0.21669601199999999</v>
-      </c>
-      <c r="D8">
-        <v>7.7646688000000005E-2</v>
-      </c>
-      <c r="E8">
-        <v>575</v>
-      </c>
-      <c r="F8">
-        <v>2.7907952869999999</v>
-      </c>
-      <c r="G8">
-        <v>1.4991436E-2</v>
-      </c>
-      <c r="H8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9">
-        <v>0.281123489</v>
-      </c>
-      <c r="D9">
-        <v>7.7646688000000005E-2</v>
-      </c>
-      <c r="E9">
-        <v>575</v>
-      </c>
-      <c r="F9">
-        <v>3.620547052</v>
-      </c>
-      <c r="G9">
-        <v>9.3213699999999998E-4</v>
-      </c>
-      <c r="H9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10">
-        <v>6.4427476999999997E-2</v>
-      </c>
-      <c r="D10">
-        <v>7.7646688000000005E-2</v>
-      </c>
-      <c r="E10">
-        <v>575</v>
-      </c>
-      <c r="F10">
-        <v>0.82975176500000003</v>
-      </c>
-      <c r="G10">
-        <v>0.68469282799999998</v>
-      </c>
-      <c r="H10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11">
-        <v>8.5700772080000007</v>
-      </c>
-      <c r="D11">
-        <v>9.7223171730000004</v>
-      </c>
-      <c r="E11">
-        <v>575</v>
-      </c>
-      <c r="F11">
-        <v>0.88148504699999997</v>
-      </c>
-      <c r="G11">
-        <v>0.65221859699999996</v>
-      </c>
-      <c r="H11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12">
-        <v>12.40503958</v>
-      </c>
-      <c r="D12">
-        <v>9.7223171730000004</v>
-      </c>
-      <c r="E12">
-        <v>575</v>
-      </c>
-      <c r="F12">
-        <v>1.2759344669999999</v>
-      </c>
-      <c r="G12">
-        <v>0.40936276799999999</v>
-      </c>
-      <c r="H12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13">
-        <v>3.8349623689999999</v>
-      </c>
-      <c r="D13">
-        <v>9.7223171730000004</v>
-      </c>
-      <c r="E13">
-        <v>575</v>
-      </c>
-      <c r="F13">
-        <v>0.39444942</v>
-      </c>
-      <c r="G13">
-        <v>0.91783244600000002</v>
-      </c>
-      <c r="H13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14">
-        <v>1.8168878580000001</v>
-      </c>
-      <c r="D14">
-        <v>0.57008712699999997</v>
-      </c>
-      <c r="E14">
-        <v>575</v>
-      </c>
-      <c r="F14">
-        <v>3.187035405</v>
-      </c>
-      <c r="G14">
-        <v>4.3177270000000004E-3</v>
-      </c>
-      <c r="H14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15">
-        <v>2.0088078039999999</v>
-      </c>
-      <c r="D15">
-        <v>0.57008712699999997</v>
-      </c>
-      <c r="E15">
-        <v>575</v>
-      </c>
-      <c r="F15">
-        <v>3.5236856059999999</v>
-      </c>
-      <c r="G15">
-        <v>1.333112E-3</v>
-      </c>
-      <c r="H15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16">
-        <v>0.19191994600000001</v>
-      </c>
-      <c r="D16">
-        <v>0.57008712699999997</v>
-      </c>
-      <c r="E16">
-        <v>575</v>
-      </c>
-      <c r="F16">
-        <v>0.33665020099999998</v>
-      </c>
-      <c r="G16">
-        <v>0.93944859599999997</v>
-      </c>
-      <c r="H16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17">
-        <v>-4.4100175019999996</v>
-      </c>
-      <c r="D17">
-        <v>1.308326594</v>
-      </c>
-      <c r="E17">
-        <v>575</v>
-      </c>
-      <c r="F17">
-        <v>-3.3707313769999998</v>
-      </c>
-      <c r="G17">
-        <v>2.3040999999999999E-3</v>
-      </c>
-      <c r="H17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18">
-        <v>-7.2723542490000002</v>
-      </c>
-      <c r="D18">
-        <v>1.308326594</v>
-      </c>
-      <c r="E18">
-        <v>575</v>
-      </c>
-      <c r="F18">
-        <v>-5.5585159559999999</v>
-      </c>
-      <c r="G18" s="1">
-        <v>1.2499999999999999E-7</v>
-      </c>
-      <c r="H18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19">
-        <v>-2.862336746</v>
-      </c>
-      <c r="D19">
-        <v>1.308326594</v>
-      </c>
-      <c r="E19">
-        <v>575</v>
-      </c>
-      <c r="F19">
-        <v>-2.1877845790000001</v>
-      </c>
-      <c r="G19">
-        <v>7.4114450999999998E-2</v>
-      </c>
-      <c r="H19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20">
-        <v>4.769230769</v>
-      </c>
-      <c r="D20">
-        <v>9.5136111840000002</v>
-      </c>
-      <c r="E20">
-        <v>575</v>
-      </c>
-      <c r="F20">
-        <v>0.50130604199999995</v>
-      </c>
-      <c r="G20">
-        <v>0.87070999900000001</v>
-      </c>
-      <c r="H20" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21">
-        <v>6.461538462</v>
-      </c>
-      <c r="D21">
-        <v>9.5136111840000002</v>
-      </c>
-      <c r="E21">
-        <v>575</v>
-      </c>
-      <c r="F21">
-        <v>0.67918883100000005</v>
-      </c>
-      <c r="G21">
-        <v>0.77571718999999995</v>
-      </c>
-      <c r="H21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22">
-        <v>1.692307692</v>
-      </c>
-      <c r="D22">
-        <v>9.5136111840000002</v>
-      </c>
-      <c r="E22">
-        <v>575</v>
-      </c>
-      <c r="F22">
-        <v>0.17788278900000001</v>
-      </c>
-      <c r="G22">
-        <v>0.98270765100000002</v>
-      </c>
-      <c r="H22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="G2:G22">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="lessThan">
-      <formula>0.001</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="between">
-      <formula>0.01</formula>
-      <formula>0.001</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="between">
       <formula>0.05</formula>
       <formula>0.01</formula>
     </cfRule>

</xml_diff>